<commit_message>
updated stop training logic
</commit_message>
<xml_diff>
--- a/assets/TrainingResults.xlsx
+++ b/assets/TrainingResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\OwenEC\Projects\InvoiceAssembly\InvoiceAssembly\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\OwenEC\Projects\InvoiceAssembly\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5682BED9-8A5B-4C58-8B7B-C06E7F7A3A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696EFDB6-8D97-4161-A4C0-B96A5C4CA4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="16020" windowWidth="29040" windowHeight="15720" xr2:uid="{0FE2DF79-3EF5-4D01-A58C-B5938D789899}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Training Loss</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Session 3</t>
   </si>
 </sst>
 </file>
@@ -225,8 +228,104 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB9B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB9B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB9B9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB9B9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -555,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED80992-2FC7-426C-8277-D9971CBF438E}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C12"/>
+      <selection activeCell="A14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,12 +865,129 @@
         <v>-1.8481668950711301E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.19826299999999999</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.1052</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.12718599999999999</v>
+      </c>
+      <c r="D16" s="4">
+        <f>(B15-B16)/B15</f>
+        <v>0.23490909090909096</v>
+      </c>
+      <c r="E16" s="4">
+        <f>(C15-C16)/C15</f>
+        <v>0.35849855999354396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4">
+        <f t="shared" ref="D17:D18" si="4">(B16-B17)/B16</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" ref="E17:E18" si="5">(C16-C17)/C16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C3:C6">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C12">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>$B$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>$B$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>